<commit_message>
- Trying to solve auto logout issue. - Edit feature added for reports(as a new child report) - Assistants is now working. (a minor bug in UI stil exists)
</commit_message>
<xml_diff>
--- a/VinarishMvc/wwwroot/Excel/LostReports.xlsx
+++ b/VinarishMvc/wwwroot/Excel/LostReports.xlsx
@@ -12,192 +12,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="540">
   <si>
     <t>شماره ردیف</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>32</t>
-  </si>
-  <si>
     <t>33</t>
   </si>
   <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>41</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>47</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>52</t>
+    <t>35</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>56</t>
-  </si>
-  <si>
     <t>57</t>
   </si>
   <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>63</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>65</t>
-  </si>
-  <si>
-    <t>66</t>
+    <t>69</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>76</t>
   </si>
   <si>
     <t>77</t>
   </si>
   <si>
+    <t>79</t>
+  </si>
+  <si>
     <t>82</t>
   </si>
   <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>88</t>
+    <t>83</t>
   </si>
   <si>
     <t>89</t>
   </si>
   <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>104</t>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>103</t>
   </si>
   <si>
     <t>105</t>
   </si>
   <si>
-    <t>111</t>
+    <t>108</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>112</t>
   </si>
   <si>
     <t>114</t>
   </si>
   <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
     <t>121</t>
   </si>
   <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>127</t>
+    <t>122</t>
   </si>
   <si>
     <t>128</t>
   </si>
   <si>
-    <t>134</t>
+    <t>133</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
   </si>
   <si>
     <t>137</t>
   </si>
   <si>
-    <t>138</t>
-  </si>
-  <si>
     <t>139</t>
   </si>
   <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>145</t>
+    <t>143</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>149</t>
   </si>
   <si>
     <t>150</t>
@@ -206,66 +155,78 @@
     <t>152</t>
   </si>
   <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>164</t>
-  </si>
-  <si>
-    <t>167</t>
+    <t>153</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>169</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>171</t>
+  </si>
+  <si>
+    <t>172</t>
   </si>
   <si>
     <t>175</t>
   </si>
   <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
     <t>184</t>
   </si>
   <si>
-    <t>189</t>
-  </si>
-  <si>
-    <t>191</t>
+    <t>188</t>
   </si>
   <si>
     <t>192</t>
   </si>
   <si>
+    <t>195</t>
+  </si>
+  <si>
     <t>196</t>
   </si>
   <si>
-    <t>199</t>
+    <t>197</t>
+  </si>
+  <si>
+    <t>198</t>
   </si>
   <si>
     <t>201</t>
   </si>
   <si>
-    <t>208</t>
-  </si>
-  <si>
-    <t>219</t>
+    <t>202</t>
+  </si>
+  <si>
+    <t>209</t>
   </si>
   <si>
     <t>220</t>
   </si>
   <si>
-    <t>223</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
-    <t>226</t>
-  </si>
-  <si>
-    <t>228</t>
-  </si>
-  <si>
-    <t>230</t>
+    <t>227</t>
   </si>
   <si>
     <t>233</t>
   </si>
   <si>
+    <t>236</t>
+  </si>
+  <si>
     <t>237</t>
   </si>
   <si>
@@ -275,25 +236,19 @@
     <t>240</t>
   </si>
   <si>
+    <t>241</t>
+  </si>
+  <si>
     <t>244</t>
   </si>
   <si>
-    <t>246</t>
-  </si>
-  <si>
-    <t>248</t>
-  </si>
-  <si>
-    <t>250</t>
-  </si>
-  <si>
-    <t>257</t>
-  </si>
-  <si>
-    <t>258</t>
-  </si>
-  <si>
-    <t>262</t>
+    <t>251</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>267</t>
   </si>
   <si>
     <t>268</t>
@@ -302,64 +257,43 @@
     <t>271</t>
   </si>
   <si>
-    <t>272</t>
-  </si>
-  <si>
-    <t>276</t>
-  </si>
-  <si>
-    <t>277</t>
-  </si>
-  <si>
-    <t>282</t>
-  </si>
-  <si>
-    <t>283</t>
-  </si>
-  <si>
-    <t>285</t>
-  </si>
-  <si>
-    <t>289</t>
-  </si>
-  <si>
-    <t>290</t>
-  </si>
-  <si>
-    <t>298</t>
-  </si>
-  <si>
-    <t>299</t>
-  </si>
-  <si>
-    <t>302</t>
+    <t>273</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>287</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>294</t>
+  </si>
+  <si>
+    <t>296</t>
+  </si>
+  <si>
+    <t>300</t>
   </si>
   <si>
     <t>303</t>
   </si>
   <si>
-    <t>305</t>
+    <t>304</t>
   </si>
   <si>
     <t>307</t>
   </si>
   <si>
-    <t>309</t>
-  </si>
-  <si>
     <t>311</t>
   </si>
   <si>
-    <t>312</t>
-  </si>
-  <si>
-    <t>314</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>321</t>
+    <t>324</t>
+  </si>
+  <si>
+    <t>325</t>
   </si>
   <si>
     <t>329</t>
@@ -371,55 +305,58 @@
     <t>331</t>
   </si>
   <si>
+    <t>332</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>335</t>
+  </si>
+  <si>
     <t>336</t>
   </si>
   <si>
-    <t>339</t>
-  </si>
-  <si>
-    <t>342</t>
-  </si>
-  <si>
-    <t>343</t>
+    <t>337</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>341</t>
   </si>
   <si>
     <t>346</t>
   </si>
   <si>
-    <t>348</t>
-  </si>
-  <si>
-    <t>349</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>351</t>
-  </si>
-  <si>
     <t>352</t>
   </si>
   <si>
-    <t>353</t>
-  </si>
-  <si>
-    <t>354</t>
-  </si>
-  <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>364</t>
-  </si>
-  <si>
-    <t>365</t>
-  </si>
-  <si>
-    <t>369</t>
-  </si>
-  <si>
-    <t>370</t>
+    <t>355</t>
+  </si>
+  <si>
+    <t>357</t>
+  </si>
+  <si>
+    <t>366</t>
+  </si>
+  <si>
+    <t>372</t>
+  </si>
+  <si>
+    <t>373</t>
+  </si>
+  <si>
+    <t>374</t>
+  </si>
+  <si>
+    <t>375</t>
+  </si>
+  <si>
+    <t>376</t>
   </si>
   <si>
     <t>377</t>
@@ -428,198 +365,183 @@
     <t>380</t>
   </si>
   <si>
-    <t>384</t>
-  </si>
-  <si>
-    <t>385</t>
+    <t>381</t>
   </si>
   <si>
     <t>386</t>
   </si>
   <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>401</t>
-  </si>
-  <si>
-    <t>409</t>
-  </si>
-  <si>
-    <t>416</t>
+    <t>392</t>
+  </si>
+  <si>
+    <t>396</t>
+  </si>
+  <si>
+    <t>402</t>
+  </si>
+  <si>
+    <t>403</t>
+  </si>
+  <si>
+    <t>406</t>
+  </si>
+  <si>
+    <t>407</t>
+  </si>
+  <si>
+    <t>408</t>
+  </si>
+  <si>
+    <t>412</t>
+  </si>
+  <si>
+    <t>415</t>
   </si>
   <si>
     <t>417</t>
   </si>
   <si>
-    <t>430</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
-    <t>440</t>
-  </si>
-  <si>
-    <t>442</t>
-  </si>
-  <si>
-    <t>445</t>
-  </si>
-  <si>
-    <t>446</t>
-  </si>
-  <si>
-    <t>447</t>
-  </si>
-  <si>
-    <t>450</t>
-  </si>
-  <si>
-    <t>451</t>
-  </si>
-  <si>
-    <t>452</t>
-  </si>
-  <si>
-    <t>453</t>
-  </si>
-  <si>
-    <t>456</t>
-  </si>
-  <si>
-    <t>459</t>
-  </si>
-  <si>
-    <t>461</t>
-  </si>
-  <si>
-    <t>472</t>
-  </si>
-  <si>
-    <t>478</t>
-  </si>
-  <si>
-    <t>479</t>
-  </si>
-  <si>
-    <t>483</t>
-  </si>
-  <si>
-    <t>484</t>
-  </si>
-  <si>
-    <t>485</t>
+    <t>421</t>
+  </si>
+  <si>
+    <t>424</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t>465</t>
+  </si>
+  <si>
+    <t>469</t>
+  </si>
+  <si>
+    <t>476</t>
+  </si>
+  <si>
+    <t>477</t>
+  </si>
+  <si>
+    <t>487</t>
   </si>
   <si>
     <t>488</t>
   </si>
   <si>
-    <t>492</t>
+    <t>490</t>
+  </si>
+  <si>
+    <t>491</t>
   </si>
   <si>
     <t>495</t>
   </si>
   <si>
+    <t>496</t>
+  </si>
+  <si>
     <t>500</t>
   </si>
   <si>
     <t>501</t>
   </si>
   <si>
-    <t>506</t>
-  </si>
-  <si>
-    <t>507</t>
-  </si>
-  <si>
-    <t>508</t>
-  </si>
-  <si>
-    <t>509</t>
-  </si>
-  <si>
-    <t>512</t>
-  </si>
-  <si>
-    <t>518</t>
+    <t>502</t>
+  </si>
+  <si>
+    <t>513</t>
+  </si>
+  <si>
+    <t>515</t>
   </si>
   <si>
     <t>519</t>
   </si>
   <si>
-    <t>525</t>
-  </si>
-  <si>
-    <t>536</t>
-  </si>
-  <si>
-    <t>542</t>
-  </si>
-  <si>
-    <t>544</t>
-  </si>
-  <si>
-    <t>556</t>
-  </si>
-  <si>
-    <t>557</t>
-  </si>
-  <si>
-    <t>559</t>
-  </si>
-  <si>
-    <t>561</t>
-  </si>
-  <si>
-    <t>566</t>
-  </si>
-  <si>
-    <t>568</t>
-  </si>
-  <si>
-    <t>577</t>
+    <t>538</t>
+  </si>
+  <si>
+    <t>539</t>
+  </si>
+  <si>
+    <t>540</t>
+  </si>
+  <si>
+    <t>545</t>
+  </si>
+  <si>
+    <t>546</t>
+  </si>
+  <si>
+    <t>547</t>
+  </si>
+  <si>
+    <t>551</t>
+  </si>
+  <si>
+    <t>555</t>
+  </si>
+  <si>
+    <t>558</t>
+  </si>
+  <si>
+    <t>564</t>
+  </si>
+  <si>
+    <t>570</t>
+  </si>
+  <si>
+    <t>574</t>
+  </si>
+  <si>
+    <t>575</t>
+  </si>
+  <si>
+    <t>579</t>
+  </si>
+  <si>
+    <t>580</t>
+  </si>
+  <si>
+    <t>582</t>
   </si>
   <si>
     <t>583</t>
   </si>
   <si>
-    <t>584</t>
-  </si>
-  <si>
-    <t>585</t>
-  </si>
-  <si>
-    <t>586</t>
-  </si>
-  <si>
-    <t>587</t>
-  </si>
-  <si>
     <t>588</t>
   </si>
   <si>
-    <t>591</t>
-  </si>
-  <si>
-    <t>592</t>
+    <t>589</t>
+  </si>
+  <si>
+    <t>593</t>
+  </si>
+  <si>
+    <t>594</t>
+  </si>
+  <si>
+    <t>595</t>
+  </si>
+  <si>
+    <t>596</t>
   </si>
   <si>
     <t>597</t>
   </si>
   <si>
-    <t>600</t>
+    <t>598</t>
+  </si>
+  <si>
+    <t>602</t>
+  </si>
+  <si>
+    <t>604</t>
   </si>
   <si>
     <t>607</t>
   </si>
   <si>
-    <t>608</t>
-  </si>
-  <si>
-    <t>613</t>
-  </si>
-  <si>
     <t>614</t>
   </si>
   <si>
@@ -629,34 +551,1087 @@
     <t>620</t>
   </si>
   <si>
-    <t>626</t>
+    <t>622</t>
+  </si>
+  <si>
+    <t>623</t>
   </si>
   <si>
     <t>627</t>
   </si>
   <si>
+    <t>629</t>
+  </si>
+  <si>
+    <t>630</t>
+  </si>
+  <si>
+    <t>631</t>
+  </si>
+  <si>
+    <t>632</t>
+  </si>
+  <si>
     <t>633</t>
   </si>
   <si>
-    <t>640</t>
-  </si>
-  <si>
-    <t>642</t>
-  </si>
-  <si>
-    <t>643</t>
-  </si>
-  <si>
-    <t>644</t>
-  </si>
-  <si>
-    <t>645</t>
+    <t>635</t>
   </si>
   <si>
     <t>646</t>
   </si>
   <si>
     <t>647</t>
+  </si>
+  <si>
+    <t>648</t>
+  </si>
+  <si>
+    <t>649</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>651</t>
+  </si>
+  <si>
+    <t>652</t>
+  </si>
+  <si>
+    <t>653</t>
+  </si>
+  <si>
+    <t>654</t>
+  </si>
+  <si>
+    <t>655</t>
+  </si>
+  <si>
+    <t>656</t>
+  </si>
+  <si>
+    <t>657</t>
+  </si>
+  <si>
+    <t>658</t>
+  </si>
+  <si>
+    <t>659</t>
+  </si>
+  <si>
+    <t>660</t>
+  </si>
+  <si>
+    <t>661</t>
+  </si>
+  <si>
+    <t>662</t>
+  </si>
+  <si>
+    <t>663</t>
+  </si>
+  <si>
+    <t>664</t>
+  </si>
+  <si>
+    <t>665</t>
+  </si>
+  <si>
+    <t>666</t>
+  </si>
+  <si>
+    <t>667</t>
+  </si>
+  <si>
+    <t>668</t>
+  </si>
+  <si>
+    <t>669</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>671</t>
+  </si>
+  <si>
+    <t>672</t>
+  </si>
+  <si>
+    <t>673</t>
+  </si>
+  <si>
+    <t>674</t>
+  </si>
+  <si>
+    <t>675</t>
+  </si>
+  <si>
+    <t>676</t>
+  </si>
+  <si>
+    <t>677</t>
+  </si>
+  <si>
+    <t>678</t>
+  </si>
+  <si>
+    <t>679</t>
+  </si>
+  <si>
+    <t>680</t>
+  </si>
+  <si>
+    <t>681</t>
+  </si>
+  <si>
+    <t>682</t>
+  </si>
+  <si>
+    <t>683</t>
+  </si>
+  <si>
+    <t>684</t>
+  </si>
+  <si>
+    <t>685</t>
+  </si>
+  <si>
+    <t>686</t>
+  </si>
+  <si>
+    <t>687</t>
+  </si>
+  <si>
+    <t>688</t>
+  </si>
+  <si>
+    <t>689</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t>691</t>
+  </si>
+  <si>
+    <t>692</t>
+  </si>
+  <si>
+    <t>693</t>
+  </si>
+  <si>
+    <t>694</t>
+  </si>
+  <si>
+    <t>695</t>
+  </si>
+  <si>
+    <t>696</t>
+  </si>
+  <si>
+    <t>697</t>
+  </si>
+  <si>
+    <t>698</t>
+  </si>
+  <si>
+    <t>699</t>
+  </si>
+  <si>
+    <t>700</t>
+  </si>
+  <si>
+    <t>701</t>
+  </si>
+  <si>
+    <t>702</t>
+  </si>
+  <si>
+    <t>703</t>
+  </si>
+  <si>
+    <t>704</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>706</t>
+  </si>
+  <si>
+    <t>707</t>
+  </si>
+  <si>
+    <t>708</t>
+  </si>
+  <si>
+    <t>709</t>
+  </si>
+  <si>
+    <t>710</t>
+  </si>
+  <si>
+    <t>711</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>713</t>
+  </si>
+  <si>
+    <t>714</t>
+  </si>
+  <si>
+    <t>715</t>
+  </si>
+  <si>
+    <t>716</t>
+  </si>
+  <si>
+    <t>717</t>
+  </si>
+  <si>
+    <t>718</t>
+  </si>
+  <si>
+    <t>719</t>
+  </si>
+  <si>
+    <t>720</t>
+  </si>
+  <si>
+    <t>721</t>
+  </si>
+  <si>
+    <t>722</t>
+  </si>
+  <si>
+    <t>723</t>
+  </si>
+  <si>
+    <t>724</t>
+  </si>
+  <si>
+    <t>725</t>
+  </si>
+  <si>
+    <t>726</t>
+  </si>
+  <si>
+    <t>727</t>
+  </si>
+  <si>
+    <t>728</t>
+  </si>
+  <si>
+    <t>729</t>
+  </si>
+  <si>
+    <t>730</t>
+  </si>
+  <si>
+    <t>731</t>
+  </si>
+  <si>
+    <t>732</t>
+  </si>
+  <si>
+    <t>733</t>
+  </si>
+  <si>
+    <t>734</t>
+  </si>
+  <si>
+    <t>735</t>
+  </si>
+  <si>
+    <t>736</t>
+  </si>
+  <si>
+    <t>737</t>
+  </si>
+  <si>
+    <t>738</t>
+  </si>
+  <si>
+    <t>739</t>
+  </si>
+  <si>
+    <t>740</t>
+  </si>
+  <si>
+    <t>741</t>
+  </si>
+  <si>
+    <t>742</t>
+  </si>
+  <si>
+    <t>743</t>
+  </si>
+  <si>
+    <t>744</t>
+  </si>
+  <si>
+    <t>745</t>
+  </si>
+  <si>
+    <t>746</t>
+  </si>
+  <si>
+    <t>747</t>
+  </si>
+  <si>
+    <t>748</t>
+  </si>
+  <si>
+    <t>749</t>
+  </si>
+  <si>
+    <t>750</t>
+  </si>
+  <si>
+    <t>751</t>
+  </si>
+  <si>
+    <t>752</t>
+  </si>
+  <si>
+    <t>753</t>
+  </si>
+  <si>
+    <t>754</t>
+  </si>
+  <si>
+    <t>755</t>
+  </si>
+  <si>
+    <t>756</t>
+  </si>
+  <si>
+    <t>757</t>
+  </si>
+  <si>
+    <t>758</t>
+  </si>
+  <si>
+    <t>759</t>
+  </si>
+  <si>
+    <t>760</t>
+  </si>
+  <si>
+    <t>761</t>
+  </si>
+  <si>
+    <t>762</t>
+  </si>
+  <si>
+    <t>763</t>
+  </si>
+  <si>
+    <t>764</t>
+  </si>
+  <si>
+    <t>765</t>
+  </si>
+  <si>
+    <t>766</t>
+  </si>
+  <si>
+    <t>767</t>
+  </si>
+  <si>
+    <t>768</t>
+  </si>
+  <si>
+    <t>769</t>
+  </si>
+  <si>
+    <t>770</t>
+  </si>
+  <si>
+    <t>771</t>
+  </si>
+  <si>
+    <t>772</t>
+  </si>
+  <si>
+    <t>773</t>
+  </si>
+  <si>
+    <t>774</t>
+  </si>
+  <si>
+    <t>775</t>
+  </si>
+  <si>
+    <t>776</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>778</t>
+  </si>
+  <si>
+    <t>779</t>
+  </si>
+  <si>
+    <t>780</t>
+  </si>
+  <si>
+    <t>781</t>
+  </si>
+  <si>
+    <t>782</t>
+  </si>
+  <si>
+    <t>783</t>
+  </si>
+  <si>
+    <t>784</t>
+  </si>
+  <si>
+    <t>785</t>
+  </si>
+  <si>
+    <t>786</t>
+  </si>
+  <si>
+    <t>787</t>
+  </si>
+  <si>
+    <t>788</t>
+  </si>
+  <si>
+    <t>789</t>
+  </si>
+  <si>
+    <t>790</t>
+  </si>
+  <si>
+    <t>791</t>
+  </si>
+  <si>
+    <t>792</t>
+  </si>
+  <si>
+    <t>793</t>
+  </si>
+  <si>
+    <t>794</t>
+  </si>
+  <si>
+    <t>795</t>
+  </si>
+  <si>
+    <t>796</t>
+  </si>
+  <si>
+    <t>797</t>
+  </si>
+  <si>
+    <t>798</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>802</t>
+  </si>
+  <si>
+    <t>803</t>
+  </si>
+  <si>
+    <t>804</t>
+  </si>
+  <si>
+    <t>805</t>
+  </si>
+  <si>
+    <t>806</t>
+  </si>
+  <si>
+    <t>807</t>
+  </si>
+  <si>
+    <t>808</t>
+  </si>
+  <si>
+    <t>809</t>
+  </si>
+  <si>
+    <t>810</t>
+  </si>
+  <si>
+    <t>811</t>
+  </si>
+  <si>
+    <t>812</t>
+  </si>
+  <si>
+    <t>813</t>
+  </si>
+  <si>
+    <t>814</t>
+  </si>
+  <si>
+    <t>815</t>
+  </si>
+  <si>
+    <t>816</t>
+  </si>
+  <si>
+    <t>817</t>
+  </si>
+  <si>
+    <t>818</t>
+  </si>
+  <si>
+    <t>819</t>
+  </si>
+  <si>
+    <t>820</t>
+  </si>
+  <si>
+    <t>821</t>
+  </si>
+  <si>
+    <t>822</t>
+  </si>
+  <si>
+    <t>823</t>
+  </si>
+  <si>
+    <t>824</t>
+  </si>
+  <si>
+    <t>825</t>
+  </si>
+  <si>
+    <t>826</t>
+  </si>
+  <si>
+    <t>827</t>
+  </si>
+  <si>
+    <t>828</t>
+  </si>
+  <si>
+    <t>829</t>
+  </si>
+  <si>
+    <t>830</t>
+  </si>
+  <si>
+    <t>831</t>
+  </si>
+  <si>
+    <t>832</t>
+  </si>
+  <si>
+    <t>833</t>
+  </si>
+  <si>
+    <t>834</t>
+  </si>
+  <si>
+    <t>835</t>
+  </si>
+  <si>
+    <t>836</t>
+  </si>
+  <si>
+    <t>837</t>
+  </si>
+  <si>
+    <t>838</t>
+  </si>
+  <si>
+    <t>839</t>
+  </si>
+  <si>
+    <t>840</t>
+  </si>
+  <si>
+    <t>841</t>
+  </si>
+  <si>
+    <t>842</t>
+  </si>
+  <si>
+    <t>843</t>
+  </si>
+  <si>
+    <t>844</t>
+  </si>
+  <si>
+    <t>845</t>
+  </si>
+  <si>
+    <t>846</t>
+  </si>
+  <si>
+    <t>847</t>
+  </si>
+  <si>
+    <t>848</t>
+  </si>
+  <si>
+    <t>849</t>
+  </si>
+  <si>
+    <t>850</t>
+  </si>
+  <si>
+    <t>851</t>
+  </si>
+  <si>
+    <t>852</t>
+  </si>
+  <si>
+    <t>853</t>
+  </si>
+  <si>
+    <t>854</t>
+  </si>
+  <si>
+    <t>855</t>
+  </si>
+  <si>
+    <t>856</t>
+  </si>
+  <si>
+    <t>857</t>
+  </si>
+  <si>
+    <t>858</t>
+  </si>
+  <si>
+    <t>859</t>
+  </si>
+  <si>
+    <t>860</t>
+  </si>
+  <si>
+    <t>861</t>
+  </si>
+  <si>
+    <t>862</t>
+  </si>
+  <si>
+    <t>863</t>
+  </si>
+  <si>
+    <t>864</t>
+  </si>
+  <si>
+    <t>865</t>
+  </si>
+  <si>
+    <t>866</t>
+  </si>
+  <si>
+    <t>867</t>
+  </si>
+  <si>
+    <t>868</t>
+  </si>
+  <si>
+    <t>869</t>
+  </si>
+  <si>
+    <t>870</t>
+  </si>
+  <si>
+    <t>871</t>
+  </si>
+  <si>
+    <t>872</t>
+  </si>
+  <si>
+    <t>873</t>
+  </si>
+  <si>
+    <t>874</t>
+  </si>
+  <si>
+    <t>875</t>
+  </si>
+  <si>
+    <t>876</t>
+  </si>
+  <si>
+    <t>877</t>
+  </si>
+  <si>
+    <t>878</t>
+  </si>
+  <si>
+    <t>879</t>
+  </si>
+  <si>
+    <t>880</t>
+  </si>
+  <si>
+    <t>881</t>
+  </si>
+  <si>
+    <t>882</t>
+  </si>
+  <si>
+    <t>883</t>
+  </si>
+  <si>
+    <t>884</t>
+  </si>
+  <si>
+    <t>885</t>
+  </si>
+  <si>
+    <t>886</t>
+  </si>
+  <si>
+    <t>887</t>
+  </si>
+  <si>
+    <t>888</t>
+  </si>
+  <si>
+    <t>889</t>
+  </si>
+  <si>
+    <t>890</t>
+  </si>
+  <si>
+    <t>891</t>
+  </si>
+  <si>
+    <t>892</t>
+  </si>
+  <si>
+    <t>893</t>
+  </si>
+  <si>
+    <t>894</t>
+  </si>
+  <si>
+    <t>895</t>
+  </si>
+  <si>
+    <t>896</t>
+  </si>
+  <si>
+    <t>897</t>
+  </si>
+  <si>
+    <t>898</t>
+  </si>
+  <si>
+    <t>899</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>901</t>
+  </si>
+  <si>
+    <t>902</t>
+  </si>
+  <si>
+    <t>903</t>
+  </si>
+  <si>
+    <t>904</t>
+  </si>
+  <si>
+    <t>905</t>
+  </si>
+  <si>
+    <t>906</t>
+  </si>
+  <si>
+    <t>907</t>
+  </si>
+  <si>
+    <t>908</t>
+  </si>
+  <si>
+    <t>909</t>
+  </si>
+  <si>
+    <t>910</t>
+  </si>
+  <si>
+    <t>911</t>
+  </si>
+  <si>
+    <t>912</t>
+  </si>
+  <si>
+    <t>913</t>
+  </si>
+  <si>
+    <t>914</t>
+  </si>
+  <si>
+    <t>915</t>
+  </si>
+  <si>
+    <t>916</t>
+  </si>
+  <si>
+    <t>917</t>
+  </si>
+  <si>
+    <t>918</t>
+  </si>
+  <si>
+    <t>919</t>
+  </si>
+  <si>
+    <t>920</t>
+  </si>
+  <si>
+    <t>921</t>
+  </si>
+  <si>
+    <t>922</t>
+  </si>
+  <si>
+    <t>923</t>
+  </si>
+  <si>
+    <t>924</t>
+  </si>
+  <si>
+    <t>925</t>
+  </si>
+  <si>
+    <t>926</t>
+  </si>
+  <si>
+    <t>927</t>
+  </si>
+  <si>
+    <t>928</t>
+  </si>
+  <si>
+    <t>929</t>
+  </si>
+  <si>
+    <t>930</t>
+  </si>
+  <si>
+    <t>931</t>
+  </si>
+  <si>
+    <t>932</t>
+  </si>
+  <si>
+    <t>933</t>
+  </si>
+  <si>
+    <t>934</t>
+  </si>
+  <si>
+    <t>935</t>
+  </si>
+  <si>
+    <t>936</t>
+  </si>
+  <si>
+    <t>937</t>
+  </si>
+  <si>
+    <t>938</t>
+  </si>
+  <si>
+    <t>939</t>
+  </si>
+  <si>
+    <t>940</t>
+  </si>
+  <si>
+    <t>941</t>
+  </si>
+  <si>
+    <t>942</t>
+  </si>
+  <si>
+    <t>943</t>
+  </si>
+  <si>
+    <t>944</t>
+  </si>
+  <si>
+    <t>945</t>
+  </si>
+  <si>
+    <t>946</t>
+  </si>
+  <si>
+    <t>947</t>
+  </si>
+  <si>
+    <t>948</t>
+  </si>
+  <si>
+    <t>949</t>
+  </si>
+  <si>
+    <t>950</t>
+  </si>
+  <si>
+    <t>951</t>
+  </si>
+  <si>
+    <t>952</t>
+  </si>
+  <si>
+    <t>953</t>
+  </si>
+  <si>
+    <t>954</t>
+  </si>
+  <si>
+    <t>955</t>
+  </si>
+  <si>
+    <t>956</t>
+  </si>
+  <si>
+    <t>957</t>
+  </si>
+  <si>
+    <t>958</t>
+  </si>
+  <si>
+    <t>959</t>
+  </si>
+  <si>
+    <t>960</t>
+  </si>
+  <si>
+    <t>961</t>
+  </si>
+  <si>
+    <t>962</t>
+  </si>
+  <si>
+    <t>963</t>
+  </si>
+  <si>
+    <t>964</t>
+  </si>
+  <si>
+    <t>965</t>
+  </si>
+  <si>
+    <t>966</t>
+  </si>
+  <si>
+    <t>967</t>
+  </si>
+  <si>
+    <t>968</t>
+  </si>
+  <si>
+    <t>969</t>
+  </si>
+  <si>
+    <t>970</t>
+  </si>
+  <si>
+    <t>971</t>
+  </si>
+  <si>
+    <t>972</t>
+  </si>
+  <si>
+    <t>973</t>
+  </si>
+  <si>
+    <t>974</t>
+  </si>
+  <si>
+    <t>975</t>
+  </si>
+  <si>
+    <t>976</t>
+  </si>
+  <si>
+    <t>977</t>
+  </si>
+  <si>
+    <t>978</t>
+  </si>
+  <si>
+    <t>979</t>
+  </si>
+  <si>
+    <t>980</t>
+  </si>
+  <si>
+    <t>981</t>
+  </si>
+  <si>
+    <t>982</t>
+  </si>
+  <si>
+    <t>983</t>
+  </si>
+  <si>
+    <t>984</t>
+  </si>
+  <si>
+    <t>985</t>
+  </si>
+  <si>
+    <t>986</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>988</t>
+  </si>
+  <si>
+    <t>989</t>
+  </si>
+  <si>
+    <t>990</t>
+  </si>
+  <si>
+    <t>991</t>
+  </si>
+  <si>
+    <t>992</t>
+  </si>
+  <si>
+    <t>993</t>
+  </si>
+  <si>
+    <t>994</t>
+  </si>
+  <si>
+    <t>995</t>
+  </si>
+  <si>
+    <t>996</t>
+  </si>
+  <si>
+    <t>997</t>
   </si>
 </sst>
 </file>
@@ -702,7 +1677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A215"/>
+  <dimension ref="A1:A540"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1783,6 +2758,1631 @@
         <v>214</v>
       </c>
     </row>
+    <row r="216">
+      <c r="A216" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="0" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="0" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="0" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="0" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="0" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="0" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="0" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="0" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="0" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="0" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="0" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="0" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="0" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="0" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="0" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="0" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="0" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="0" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="0" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="0" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="0" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="0" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="0" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="0" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="0" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="0" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="0" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="0" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="0" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="0" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="0" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="0" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="0" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="0" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="0" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="0" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="0" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="0" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="0" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="0" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="0" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="0" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="0" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="0" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="0" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="0" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="0" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="0" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="0" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="0" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="0" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="0" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="0" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="0" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="0" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="0" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="0" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" s="0" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="0" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="0" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" s="0" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="0" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="0" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" s="0" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="0" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="0" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="0" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" s="0" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="0" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="0" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="0" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" s="0" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="0" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="0" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="0" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="0" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" s="0" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="0" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" s="0" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" s="0" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="0" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" s="0" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" s="0" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" s="0" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" s="0" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="0" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="0" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="0" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" s="0" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" s="0" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" s="0" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="0" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="0" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" s="0" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" s="0" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" s="0" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" s="0" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" s="0" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="0" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" s="0" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="0" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" s="0" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" s="0" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="0" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="0" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="0" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" s="0" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" s="0" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" s="0" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="0" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="0" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="0" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" s="0" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="0" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="0" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" s="0" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" s="0" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" s="0" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="0" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" s="0" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" s="0" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" s="0" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="0" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="0" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" s="0" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="0" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="0" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" s="0" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="0" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="0" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" s="0" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="0" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" s="0" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="0" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="0" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" s="0" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="0" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" s="0" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="0" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="0" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" s="0" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" s="0" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" s="0" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="0" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" s="0" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" s="0" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="0" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="0" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="0" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" s="0" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="0" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="0" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" s="0" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="0" t="s">
+        <v>539</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>